<commit_message>
customized files from tufts, downloaded 12/13
</commit_message>
<xml_diff>
--- a/InputData/elec/BCRbQ/BAU Cap Retirements before Quantization.xlsx
+++ b/InputData/elec/BCRbQ/BAU Cap Retirements before Quantization.xlsx
@@ -309,9 +309,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="10">
     <font>
       <sz val="11.0"/>
@@ -420,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -475,7 +472,6 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -12219,8 +12215,8 @@
         <f>'coal retirement'!AG3</f>
         <v>14.5</v>
       </c>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="29"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
@@ -12332,8 +12328,8 @@
       <c r="AG3" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH3" s="3"/>
-      <c r="AI3" s="29"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="28"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
@@ -12435,8 +12431,8 @@
       <c r="AG4" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH4" s="3"/>
-      <c r="AI4" s="29"/>
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="28"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="20" t="s">
@@ -12538,8 +12534,8 @@
       <c r="AG5" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="29"/>
+      <c r="AH5" s="28"/>
+      <c r="AI5" s="28"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="20" t="s">
@@ -12646,8 +12642,8 @@
       <c r="AG6" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="29"/>
+      <c r="AH6" s="28"/>
+      <c r="AI6" s="28"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="20" t="s">
@@ -12756,8 +12752,8 @@
       <c r="AG7" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="29"/>
+      <c r="AH7" s="28"/>
+      <c r="AI7" s="28"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="20" t="s">
@@ -12859,8 +12855,8 @@
       <c r="AG8" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="29"/>
+      <c r="AH8" s="28"/>
+      <c r="AI8" s="28"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="20" t="s">
@@ -12972,8 +12968,8 @@
         <f>'deploy_19-28'!C8</f>
         <v>139</v>
       </c>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="29"/>
+      <c r="AH9" s="28"/>
+      <c r="AI9" s="28"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="20" t="s">
@@ -13075,8 +13071,8 @@
       <c r="AG10" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="29"/>
+      <c r="AH10" s="28"/>
+      <c r="AI10" s="28"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="20" t="s">
@@ -13186,8 +13182,8 @@
       <c r="AG11" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="29"/>
+      <c r="AH11" s="28"/>
+      <c r="AI11" s="28"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="20" t="s">
@@ -13289,8 +13285,8 @@
       <c r="AG12" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH12" s="3"/>
-      <c r="AI12" s="29"/>
+      <c r="AH12" s="28"/>
+      <c r="AI12" s="28"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="20" t="s">
@@ -13392,8 +13388,8 @@
       <c r="AG13" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH13" s="3"/>
-      <c r="AI13" s="29"/>
+      <c r="AH13" s="28"/>
+      <c r="AI13" s="28"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="20" t="s">
@@ -13495,11 +13491,11 @@
       <c r="AG14" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH14" s="3"/>
-      <c r="AI14" s="29"/>
+      <c r="AH14" s="28"/>
+      <c r="AI14" s="28"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="20" t="s">
         <v>91</v>
       </c>
       <c r="B15" s="28">
@@ -13598,11 +13594,11 @@
       <c r="AG15" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH15" s="3"/>
-      <c r="AI15" s="3"/>
+      <c r="AH15" s="28"/>
+      <c r="AI15" s="28"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="20" t="s">
         <v>92</v>
       </c>
       <c r="B16" s="28">
@@ -13711,11 +13707,11 @@
       <c r="AG16" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH16" s="3"/>
-      <c r="AI16" s="3"/>
+      <c r="AH16" s="28"/>
+      <c r="AI16" s="28"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="20" t="s">
         <v>93</v>
       </c>
       <c r="B17" s="28">
@@ -13784,46 +13780,46 @@
       <c r="W17" s="28">
         <v>0.0</v>
       </c>
-      <c r="X17" s="29">
+      <c r="X17" s="28">
         <f>'deploy_10-19'!C38</f>
         <v>26</v>
       </c>
-      <c r="Y17" s="29">
+      <c r="Y17" s="28">
         <f>'deploy_10-19'!D38</f>
         <v>0</v>
       </c>
-      <c r="Z17" s="29">
+      <c r="Z17" s="28">
         <f>'deploy_10-19'!E38</f>
         <v>0</v>
       </c>
-      <c r="AA17" s="29">
+      <c r="AA17" s="28">
         <f>'deploy_10-19'!F38</f>
         <v>10</v>
       </c>
-      <c r="AB17" s="29">
+      <c r="AB17" s="28">
         <v>0.0</v>
       </c>
-      <c r="AC17" s="29">
+      <c r="AC17" s="28">
         <f>'deploy_10-19'!H38</f>
         <v>0</v>
       </c>
-      <c r="AD17" s="29">
+      <c r="AD17" s="28">
         <f>'deploy_10-19'!I38</f>
         <v>0</v>
       </c>
-      <c r="AE17" s="29">
+      <c r="AE17" s="28">
         <f>'deploy_10-19'!J38</f>
         <v>0</v>
       </c>
-      <c r="AF17" s="29">
+      <c r="AF17" s="28">
         <f>'deploy_10-19'!K38</f>
         <v>0</v>
       </c>
-      <c r="AG17" s="29">
+      <c r="AG17" s="28">
         <v>0.0</v>
       </c>
-      <c r="AH17" s="3"/>
-      <c r="AI17" s="3"/>
+      <c r="AH17" s="28"/>
+      <c r="AI17" s="28"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3"/>

</xml_diff>